<commit_message>
Adding DATA tab with Data that will be fed to th tests
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxsudik/IdeaProjects/JQMax/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{777D2829-7E29-524B-9E21-643DDC2A67FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C32FE532-C525-6946-A05F-3BF73F24C2FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28800" yWindow="21020" windowWidth="28800" windowHeight="25340" xr2:uid="{525FE1C0-3A4D-6640-97FF-4AA153153C6A}"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
+    <sheet name="DATA" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="26">
   <si>
     <t>testname</t>
   </si>
@@ -67,6 +68,51 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>fname</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>loginTestUsingExcelData</t>
+  </si>
+  <si>
+    <t>newTestUsingExcelData</t>
+  </si>
+  <si>
+    <t>To check import of data from excel</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Admin123</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>admin123</t>
+  </si>
+  <si>
+    <t>admin1234</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>John</t>
   </si>
 </sst>
 </file>
@@ -419,13 +465,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{806BC977-A81A-5C41-B9ED-6102EAE8A628}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="51" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
@@ -457,7 +505,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>10</v>
@@ -474,13 +522,188 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FA8BD40-08E3-F44D-AE0C-BE9D604A2C43}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView zoomScale="260" zoomScaleNormal="260" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removing parameters from @Test in order to use annotation transformer
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxsudik/IdeaProjects/JQMax/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C32FE532-C525-6946-A05F-3BF73F24C2FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1121027A-A2B1-5F49-8BA8-44D4A34EF0E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="21020" windowWidth="28800" windowHeight="25340" xr2:uid="{525FE1C0-3A4D-6640-97FF-4AA153153C6A}"/>
+    <workbookView xWindow="-28800" yWindow="21020" windowWidth="28800" windowHeight="25340" activeTab="1" xr2:uid="{525FE1C0-3A4D-6640-97FF-4AA153153C6A}"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
@@ -467,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{806BC977-A81A-5C41-B9ED-6102EAE8A628}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -505,7 +505,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>10</v>
@@ -522,7 +522,7 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>10</v>
@@ -574,8 +574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FA8BD40-08E3-F44D-AE0C-BE9D604A2C43}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView zoomScale="260" zoomScaleNormal="260" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" zoomScale="260" zoomScaleNormal="260" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Adding column to the test cases with browser name
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxsudik/IdeaProjects/JQMax/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1121027A-A2B1-5F49-8BA8-44D4A34EF0E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F0D56FA-2833-F149-A630-BB5BF1C63E8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28800" yWindow="21020" windowWidth="28800" windowHeight="25340" activeTab="1" xr2:uid="{525FE1C0-3A4D-6640-97FF-4AA153153C6A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="29">
   <si>
     <t>testname</t>
   </si>
@@ -113,6 +113,15 @@
   </si>
   <si>
     <t>John</t>
+  </si>
+  <si>
+    <t>browser</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>firefox</t>
   </si>
 </sst>
 </file>
@@ -572,22 +581,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FA8BD40-08E3-F44D-AE0C-BE9D604A2C43}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="260" zoomScaleNormal="260" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:E6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.5" customWidth="1"/>
+    <col min="3" max="3" width="7.5" customWidth="1"/>
+    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -595,16 +605,19 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -612,16 +625,19 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
         <v>18</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>21</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -637,8 +653,11 @@
       <c r="E3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -646,16 +665,19 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
         <v>19</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>22</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -671,8 +693,11 @@
       <c r="E5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -680,16 +705,19 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
         <v>18</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>21</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -703,6 +731,9 @@
         <v>20</v>
       </c>
       <c r="E7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactoring exception handling in the framework classes
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxsudik/IdeaProjects/JQMax/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F0D56FA-2833-F149-A630-BB5BF1C63E8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3353014B-C4CE-8640-9C45-7E39E9B9E9EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28800" yWindow="21020" windowWidth="28800" windowHeight="25340" activeTab="1" xr2:uid="{525FE1C0-3A4D-6640-97FF-4AA153153C6A}"/>
   </bookViews>
@@ -477,7 +477,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -584,7 +584,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="260" zoomScaleNormal="260" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -662,7 +662,7 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
         <v>28</v>
@@ -702,7 +702,7 @@
         <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
Adding version column to DATA in order to implement browser compatibility testing
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxsudik/IdeaProjects/JQMax/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3353014B-C4CE-8640-9C45-7E39E9B9E9EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B29144-6A6C-2848-AC32-C0E10634C5E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28800" yWindow="21020" windowWidth="28800" windowHeight="25340" activeTab="1" xr2:uid="{525FE1C0-3A4D-6640-97FF-4AA153153C6A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="30">
   <si>
     <t>testname</t>
   </si>
@@ -122,6 +122,9 @@
   </si>
   <si>
     <t>firefox</t>
+  </si>
+  <si>
+    <t>version</t>
   </si>
 </sst>
 </file>
@@ -581,23 +584,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FA8BD40-08E3-F44D-AE0C-BE9D604A2C43}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="260" zoomScaleNormal="260" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D2" sqref="D2:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5" customWidth="1"/>
-    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.5" customWidth="1"/>
+    <col min="3" max="4" width="7.5" customWidth="1"/>
+    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -608,16 +611,19 @@
         <v>26</v>
       </c>
       <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -628,16 +634,19 @@
         <v>27</v>
       </c>
       <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>21</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -656,8 +665,11 @@
       <c r="F3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -668,16 +680,19 @@
         <v>28</v>
       </c>
       <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
         <v>19</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>22</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -696,8 +711,11 @@
       <c r="F5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -708,16 +726,19 @@
         <v>28</v>
       </c>
       <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
         <v>18</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>21</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -734,6 +755,9 @@
         <v>20</v>
       </c>
       <c r="F7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding column with versions of browsers to use in docker containers
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxsudik/IdeaProjects/JQMax/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B29144-6A6C-2848-AC32-C0E10634C5E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4976CBD-72A3-8B4C-BA2B-B761D06C96AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28800" yWindow="21020" windowWidth="28800" windowHeight="25340" activeTab="1" xr2:uid="{525FE1C0-3A4D-6640-97FF-4AA153153C6A}"/>
   </bookViews>
@@ -79,52 +79,52 @@
     <t>fname</t>
   </si>
   <si>
+    <t>loginTestUsingExcelData</t>
+  </si>
+  <si>
+    <t>newTestUsingExcelData</t>
+  </si>
+  <si>
+    <t>To check import of data from excel</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>admin123</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>browser</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>firefox</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>95.0.2</t>
+  </si>
+  <si>
+    <t>Admin1</t>
+  </si>
+  <si>
     <t>no</t>
-  </si>
-  <si>
-    <t>loginTestUsingExcelData</t>
-  </si>
-  <si>
-    <t>newTestUsingExcelData</t>
-  </si>
-  <si>
-    <t>To check import of data from excel</t>
-  </si>
-  <si>
-    <t>Admin</t>
-  </si>
-  <si>
-    <t>Admin123</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>admin123</t>
-  </si>
-  <si>
-    <t>admin1234</t>
-  </si>
-  <si>
-    <t>Max</t>
-  </si>
-  <si>
-    <t>Bob</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>browser</t>
-  </si>
-  <si>
-    <t>chrome</t>
-  </si>
-  <si>
-    <t>firefox</t>
-  </si>
-  <si>
-    <t>version</t>
   </si>
 </sst>
 </file>
@@ -480,7 +480,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E5"/>
+      <selection activeCell="C5" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -545,10 +545,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -562,10 +562,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
         <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -587,7 +587,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="260" zoomScaleNormal="260" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D7"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -608,10 +608,10 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
         <v>26</v>
-      </c>
-      <c r="D1" t="s">
-        <v>29</v>
       </c>
       <c r="E1" t="s">
         <v>11</v>
@@ -625,140 +625,140 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
         <v>20</v>
-      </c>
-      <c r="E2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
+        <v>25</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s">
         <v>19</v>
       </c>
-      <c r="F4" t="s">
-        <v>22</v>
-      </c>
       <c r="G4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
         <v>28</v>
       </c>
-      <c r="D6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" t="s">
-        <v>18</v>
-      </c>
       <c r="F6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enabling all test cases in order to populate data in elastic search and kibana
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxsudik/IdeaProjects/JQMax/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4976CBD-72A3-8B4C-BA2B-B761D06C96AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84FFB96C-9BB8-0546-BC4E-6E6F06EBB1F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28800" yWindow="21020" windowWidth="28800" windowHeight="25340" activeTab="1" xr2:uid="{525FE1C0-3A4D-6640-97FF-4AA153153C6A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="29">
   <si>
     <t>testname</t>
   </si>
@@ -122,9 +122,6 @@
   </si>
   <si>
     <t>Admin1</t>
-  </si>
-  <si>
-    <t>no</t>
   </si>
 </sst>
 </file>
@@ -587,7 +584,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="260" zoomScaleNormal="260" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B2" sqref="B2:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -628,7 +625,7 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
         <v>24</v>
@@ -651,7 +648,7 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
         <v>24</v>
@@ -697,7 +694,7 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
         <v>25</v>
@@ -720,7 +717,7 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
         <v>25</v>
@@ -743,7 +740,7 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
92 fix method the creates path to the folder with reports, when reports are not override after the exec (#93)
* Fixing createReportPath() method in order to generate correct name of the folders where reports will be stored if in config it is said do not override reports

* Cleanup
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxsudik/IdeaProjects/JQMax/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84FFB96C-9BB8-0546-BC4E-6E6F06EBB1F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D67E7322-E304-AD4B-A0A5-8FA9F423DA2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28800" yWindow="21020" windowWidth="28800" windowHeight="25340" activeTab="1" xr2:uid="{525FE1C0-3A4D-6640-97FF-4AA153153C6A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="24">
   <si>
     <t>testname</t>
   </si>
@@ -76,9 +76,6 @@
     <t>password</t>
   </si>
   <si>
-    <t>fname</t>
-  </si>
-  <si>
     <t>loginTestUsingExcelData</t>
   </si>
   <si>
@@ -97,15 +94,6 @@
     <t>admin123</t>
   </si>
   <si>
-    <t>Max</t>
-  </si>
-  <si>
-    <t>Bob</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
     <t>browser</t>
   </si>
   <si>
@@ -116,9 +104,6 @@
   </si>
   <si>
     <t>version</t>
-  </si>
-  <si>
-    <t>95.0.2</t>
   </si>
   <si>
     <t>Admin1</t>
@@ -542,10 +527,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -559,10 +544,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
         <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -581,11 +566,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FA8BD40-08E3-F44D-AE0C-BE9D604A2C43}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="260" zoomScaleNormal="260" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B7"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="260" zoomScaleNormal="260" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -594,10 +577,9 @@
     <col min="3" max="4" width="7.5" customWidth="1"/>
     <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -605,10 +587,10 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E1" t="s">
         <v>11</v>
@@ -616,145 +598,124 @@
       <c r="F1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
         <v>18</v>
       </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
         <v>17</v>
       </c>
-      <c r="F2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
         <v>17</v>
       </c>
-      <c r="F4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" t="s">
-        <v>18</v>
-      </c>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>